<commit_message>
Update tracker after talking to Patrick
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A382CB-5E12-4F7C-8717-8430B7F08181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BB7A15-247C-405F-BD09-A5741C360231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18885" yWindow="2595" windowWidth="15120" windowHeight="12885" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
+    <workbookView xWindow="-16170" yWindow="0" windowWidth="16275" windowHeight="15585" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -74,13 +74,7 @@
     <t>Allow profile(_cons)?</t>
   </si>
   <si>
-    <t>Improve -rmcoll-: drop altogether or make noRMcoll the default?</t>
-  </si>
-  <si>
     <t>Update help file</t>
-  </si>
-  <si>
-    <t>ask Patrick</t>
   </si>
   <si>
     <t>"Handling 'equations' correctly" section of help file seems to be wrong. Certainly -pllf, profile(x): poisson x, exposure()- works</t>
@@ -93,9 +87,6 @@
     <t xml:space="preserve">use_deviance. Ian: only defined in the profile() part, so I removed it from formula(). Shoud it instead have been defined also for formula()? Patrick: Not sure. Suggest putting this on the back burner with the code as in the original version. It may turn up again with more intensive testing or use (?). </t>
   </si>
   <si>
-    <t>At present it drops x's that are collinear with y, which is wrong e.g. for analysis of 2x2 table</t>
-  </si>
-  <si>
     <t>Make it work with perfect prediction</t>
   </si>
   <si>
@@ -132,13 +123,55 @@
     <t>added to help file</t>
   </si>
   <si>
-    <t>discuss</t>
-  </si>
-  <si>
     <t>done, but check my defaults and add to help</t>
   </si>
   <si>
     <t>make repo public</t>
+  </si>
+  <si>
+    <t>need help file example for syntax 2</t>
+  </si>
+  <si>
+    <t>remove from help</t>
+  </si>
+  <si>
+    <t>change !mi to !missing passim</t>
+  </si>
+  <si>
+    <t>help file should note this difference</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>pllf, formula(exp(-X*x5)) range(-3 -1): stcox x1 x4a X x6 hormon</t>
+  </si>
+  <si>
+    <t>pllf, profile(_cons) n(50): streg x1 x4a x5e x6 hormon, distribution(weibull)</t>
+  </si>
+  <si>
+    <t>syntax 1 example for profiling constant - use brca data</t>
+  </si>
+  <si>
+    <t>document mleline and DROPCollinear</t>
+  </si>
+  <si>
+    <t>authors: Patrick, Ian, Ian email</t>
+  </si>
+  <si>
+    <t>find example for syntax 1: TBCHAMP / TRISST - to help file?</t>
+  </si>
+  <si>
+    <t>and use in talk!</t>
+  </si>
+  <si>
+    <t>tbd later</t>
+  </si>
+  <si>
+    <t>yes worth doing: -shownormal- option</t>
+  </si>
+  <si>
+    <t>explore TRISST example in n:</t>
   </si>
 </sst>
 </file>
@@ -174,12 +207,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -220,8 +256,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E18" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E18" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E24" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E24" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BB16AB2A-B854-4B63-A177-54B619CECB81}" name="problem" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{55DC27BD-1A0D-41AE-9DC9-2CF3279076C1}" name="Raised by" dataDxfId="3"/>
@@ -550,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,10 +611,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -587,35 +623,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
-        <v>45826</v>
+        <v>45806</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
         <v>45826</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2">
-        <v>45826</v>
+        <v>45806</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2">
         <v>45826</v>
@@ -623,10 +659,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>45806</v>
@@ -638,18 +674,18 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2">
         <v>45806</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
         <v>45826</v>
@@ -657,16 +693,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2">
         <v>45806</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2">
         <v>45826</v>
@@ -674,10 +710,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2">
         <v>45806</v>
@@ -686,156 +722,248 @@
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>45826</v>
+        <v>45856</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>45806</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
+      <c r="D9" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2">
         <v>45806</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E10" s="2">
-        <v>45856</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>45826</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2">
         <v>45806</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="2">
-        <v>45806</v>
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2">
-        <v>45826</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2">
-        <v>45806</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>45826</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>45826</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45826</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
+      <c r="E14" s="2">
+        <v>45861</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2">
         <v>45826</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45826</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45856</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2">
-        <v>45826</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="2">
-        <v>45826</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="2">
-        <v>45856</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
+      <c r="C19" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
+        <v>45868</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New shownormal option, and fix stpm and noconstant
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BB7A15-247C-405F-BD09-A5741C360231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5CB01F-DD22-472A-BB22-82A23083F9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16170" yWindow="0" windowWidth="16275" windowHeight="15585" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
+    <workbookView xWindow="-60" yWindow="60" windowWidth="20715" windowHeight="14820" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -138,9 +138,6 @@
     <t>change !mi to !missing passim</t>
   </si>
   <si>
-    <t>help file should note this difference</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -172,6 +169,15 @@
   </si>
   <si>
     <t>explore TRISST example in n:</t>
+  </si>
+  <si>
+    <t>does pllf handle break correctly?</t>
+  </si>
+  <si>
+    <t>not sure; seem to give same answer; but constraint is faster!</t>
+  </si>
+  <si>
+    <t>yes - no action needed</t>
   </si>
 </sst>
 </file>
@@ -207,15 +213,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -256,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E24" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E24" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E25" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E25" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BB16AB2A-B854-4B63-A177-54B619CECB81}" name="problem" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{55DC27BD-1A0D-41AE-9DC9-2CF3279076C1}" name="Raised by" dataDxfId="3"/>
@@ -586,27 +589,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.54296875" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -623,7 +626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -640,7 +643,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -657,7 +660,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -674,7 +677,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -691,7 +694,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -708,7 +711,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -725,7 +728,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -735,12 +738,14 @@
       <c r="C9" s="2">
         <v>45806</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E9" s="2">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -750,14 +755,14 @@
       <c r="C10" s="2">
         <v>45806</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="2">
         <v>45826</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -768,11 +773,11 @@
         <v>45806</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -789,7 +794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -806,7 +811,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -816,14 +821,14 @@
       <c r="C14" s="2">
         <v>45826</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="2">
         <v>45861</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -834,11 +839,11 @@
         <v>45826</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -849,12 +854,14 @@
         <v>45826</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="2">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -864,12 +871,12 @@
         <v>45856</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -879,11 +886,11 @@
         <v>45868</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -893,12 +900,16 @@
       <c r="C19" s="2">
         <v>45868</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
@@ -907,13 +918,13 @@
         <v>45868</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
@@ -924,9 +935,9 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
@@ -934,12 +945,16 @@
       <c r="C22" s="2">
         <v>45868</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
@@ -948,13 +963,13 @@
         <v>45868</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -964,6 +979,23 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="2">
+        <v>45869</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="2">
+        <v>45870</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Document new options, improve examples and add TRISST example
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5CB01F-DD22-472A-BB22-82A23083F9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1CB881-4AEF-408D-9FB5-51ED6F17FC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="60" windowWidth="20715" windowHeight="14820" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20715" windowHeight="14820" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -141,12 +141,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>pllf, formula(exp(-X*x5)) range(-3 -1): stcox x1 x4a X x6 hormon</t>
-  </si>
-  <si>
-    <t>pllf, profile(_cons) n(50): streg x1 x4a x5e x6 hormon, distribution(weibull)</t>
-  </si>
-  <si>
     <t>syntax 1 example for profiling constant - use brca data</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>yes worth doing: -shownormal- option</t>
   </si>
   <si>
-    <t>explore TRISST example in n:</t>
-  </si>
-  <si>
     <t>does pllf handle break correctly?</t>
   </si>
   <si>
@@ -178,6 +169,12 @@
   </si>
   <si>
     <t>yes - no action needed</t>
+  </si>
+  <si>
+    <t>should the last estimation command be dropped from memory?</t>
+  </si>
+  <si>
+    <t>discuss</t>
   </si>
 </sst>
 </file>
@@ -591,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +770,7 @@
         <v>45806</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -839,7 +836,7 @@
         <v>45826</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -854,7 +851,7 @@
         <v>45826</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2">
         <v>45870</v>
@@ -875,7 +872,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -886,9 +883,11 @@
         <v>45868</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>45870</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -907,9 +906,9 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
@@ -918,13 +917,15 @@
         <v>45868</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <v>45870</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
@@ -932,12 +933,16 @@
       <c r="C21" s="2">
         <v>45868</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>45870</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
@@ -954,7 +959,7 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
@@ -963,24 +968,30 @@
         <v>45868</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E23" s="2">
+        <v>45870</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
+        <v>45869</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2">
-        <v>45868</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="2">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -988,14 +999,12 @@
         <v>23</v>
       </c>
       <c r="C25" s="2">
-        <v>45869</v>
+        <v>45870</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="2">
-        <v>45870</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates after talking to Patrick
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1CB881-4AEF-408D-9FB5-51ED6F17FC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D27476-925E-4A76-AEEB-DE282E9BAFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20715" windowHeight="14820" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>discuss</t>
+  </si>
+  <si>
+    <t>save the normal approx to data?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reload the model with the selected parameter value (MLE) and leave that model in memory.  If there is no such value we just leave nothing via ereturn clear. </t>
+  </si>
+  <si>
+    <t>change first help file example from 38-19 to 8-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improve "Stored results" section - to be like -h regress-? </t>
+  </si>
+  <si>
+    <t>Improve help file by showing both syntaxes in the syntax diagram, thus also explaining what pllf does; changing the RHS of the syntax diagram to just regression_cmd</t>
+  </si>
+  <si>
+    <t>Syntax 2: Remove the placeholder X from regression_cmd; make the default placeholder(#)</t>
   </si>
 </sst>
 </file>
@@ -256,8 +274,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E25" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E25" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E30" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E30" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BB16AB2A-B854-4B63-A177-54B619CECB81}" name="problem" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{55DC27BD-1A0D-41AE-9DC9-2CF3279076C1}" name="Raised by" dataDxfId="3"/>
@@ -586,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1009,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1002,9 +1020,76 @@
         <v>45870</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2">
+        <v>45874</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="2">
+        <v>45883</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="2">
+        <v>45883</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="2">
+        <v>45883</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="2">
+        <v>45883</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor improvements to ado and help file
from IW/PR discussion 29/09/2025
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6560A89-4E4F-4909-BB72-86A7BAA30529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF0938A-BC02-46A1-B254-BD8BB4DDB898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
+    <workbookView xWindow="-26010" yWindow="2790" windowWidth="21600" windowHeight="11175" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -84,9 +84,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">use_deviance. Ian: only defined in the profile() part, so I removed it from formula(). Shoud it instead have been defined also for formula()? Patrick: Not sure. Suggest putting this on the back burner with the code as in the original version. It may turn up again with more intensive testing or use (?). </t>
-  </si>
-  <si>
     <t>Make it work with perfect prediction</t>
   </si>
   <si>
@@ -150,21 +147,9 @@
     <t>find example for syntax 1: TBCHAMP / TRISST - to help file?</t>
   </si>
   <si>
-    <t>and use in talk!</t>
-  </si>
-  <si>
-    <t>tbd later</t>
-  </si>
-  <si>
-    <t>yes worth doing: -shownormal- option</t>
-  </si>
-  <si>
     <t>does pllf handle break correctly?</t>
   </si>
   <si>
-    <t>not sure; seem to give same answer; but constraint is faster!</t>
-  </si>
-  <si>
     <t>yes - no action needed</t>
   </si>
   <si>
@@ -183,18 +168,12 @@
     <t>test pllf when there are interactions in the model</t>
   </si>
   <si>
-    <t>it only works at present using xi</t>
-  </si>
-  <si>
     <t>save the normal approx to data</t>
   </si>
   <si>
     <t>Syntax 2: Remove the placeholder X from regression_cmd; make the default placeholder(@)</t>
   </si>
   <si>
-    <t>ereturn clear</t>
-  </si>
-  <si>
     <t>why are the Pearce and Venzon references in the help file? Omit?</t>
   </si>
   <si>
@@ -214,6 +193,39 @@
   </si>
   <si>
     <t>help file: default was 16000 in Stata 13, but is 300 now</t>
+  </si>
+  <si>
+    <t>try to make it work for syntax 2</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>it only works at present using xi - put in help file</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>state as limitation</t>
+  </si>
+  <si>
+    <t>print warning but run anyway</t>
+  </si>
+  <si>
+    <t>change to "many" and mention iter() option</t>
+  </si>
+  <si>
+    <t>"The term "profile" implies adjustment for other predictor(s) in the model, if any" is not quite correct</t>
+  </si>
+  <si>
+    <t>ereturn clear - done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_deviance. Ian: only defined in the profile() part, so I removed it from formula(). Should it instead have been defined also for formula()? Patrick: Not sure. Suggest putting this on the back burner with the code as in the original version. It may turn up again with more intensive testing or use (?). </t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -295,12 +307,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E38" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E38" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}">
-    <filterColumn colId="4">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E39" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E39" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BB16AB2A-B854-4B63-A177-54B619CECB81}" name="problem" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{55DC27BD-1A0D-41AE-9DC9-2CF3279076C1}" name="Raised by" dataDxfId="3"/>
@@ -629,35 +637,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="47.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -666,12 +674,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2">
         <v>45806</v>
@@ -683,29 +691,29 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2">
         <v>45806</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2">
         <v>45826</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2">
         <v>45806</v>
@@ -717,12 +725,12 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>45806</v>
@@ -734,29 +742,29 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2">
         <v>45806</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2">
         <v>45826</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2">
         <v>45806</v>
@@ -768,78 +776,78 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2">
         <v>45806</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2">
         <v>45870</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2">
         <v>45806</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
         <v>45826</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>45806</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2">
         <v>45826</v>
@@ -851,12 +859,12 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2">
         <v>45826</v>
@@ -868,44 +876,46 @@
         <v>45861</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2">
         <v>45826</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2">
         <v>45826</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E16" s="2">
         <v>45870</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2">
         <v>45856</v>
@@ -917,12 +927,12 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2">
         <v>45868</v>
@@ -934,12 +944,12 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2">
         <v>45868</v>
@@ -951,12 +961,12 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2">
         <v>45868</v>
@@ -968,12 +978,12 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2">
         <v>45868</v>
@@ -985,12 +995,12 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2">
         <v>45868</v>
@@ -1002,63 +1012,63 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="2">
         <v>45868</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2">
         <v>45870</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2">
         <v>45869</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E24" s="2">
         <v>45870</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2">
         <v>45870</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E25" s="2">
         <v>45901</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2">
         <v>45874</v>
@@ -1070,12 +1080,12 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2">
         <v>45883</v>
@@ -1087,12 +1097,12 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="2">
         <v>45883</v>
@@ -1104,12 +1114,12 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2">
         <v>45883</v>
@@ -1121,12 +1131,12 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2">
         <v>45883</v>
@@ -1138,111 +1148,158 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2">
         <v>45888</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E31" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2">
         <v>45903</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2">
         <v>45916</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="2">
         <v>45916</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="2">
         <v>45919</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="2">
         <v>45929</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="2">
         <v>45929</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" s="2">
         <v>45929</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="2"/>
+      <c r="D38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="2">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45932</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="2">
+        <v>45964</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Better error reporting motivated by failure with mixed
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF0938A-BC02-46A1-B254-BD8BB4DDB898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C080095F-D07C-454E-9497-F9D1C6767C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26010" yWindow="2790" windowWidth="21600" windowHeight="11175" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>check whether old code worked for mixed; document that new code doesn't because neither offset nor constraint is allowed (despite the help file saying constraint is allowed), and that meglm can be tried</t>
   </si>
 </sst>
 </file>
@@ -307,8 +310,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E39" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E39" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E40" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E40" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BB16AB2A-B854-4B63-A177-54B619CECB81}" name="problem" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{55DC27BD-1A0D-41AE-9DC9-2CF3279076C1}" name="Raised by" dataDxfId="3"/>
@@ -637,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1301,6 +1304,19 @@
         <v>45964</v>
       </c>
     </row>
+    <row r="40" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45981</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Updates tests and re-run
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C080095F-D07C-454E-9497-F9D1C6767C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F66EA3E-A4A2-4B5E-B749-9D8AB2E87843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>check whether old code worked for mixed; document that new code doesn't because neither offset nor constraint is allowed (despite the help file saying constraint is allowed), and that meglm can be tried</t>
+  </si>
+  <si>
+    <t>make meglm work without rmcoll</t>
+  </si>
+  <si>
+    <t>syntax 2: expand 1st derivative to act after any collinearity</t>
   </si>
 </sst>
 </file>
@@ -310,8 +316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E40" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E40" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E42" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E42" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BB16AB2A-B854-4B63-A177-54B619CECB81}" name="problem" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{55DC27BD-1A0D-41AE-9DC9-2CF3279076C1}" name="Raised by" dataDxfId="3"/>
@@ -640,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1314,8 +1320,38 @@
       <c r="C40" s="2">
         <v>45981</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="2"/>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45985</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45985</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correctly handle me commands and collinearity tests
including syntax 2: new collinearity -> differentiate
</commit_message>
<xml_diff>
--- a/pllf-to-do.xlsx
+++ b/pllf-to-do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\pllf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F66EA3E-A4A2-4B5E-B749-9D8AB2E87843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AAF6E0-0782-4DD2-A758-B152A6F0E6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C055561-BBF2-4058-BDFC-581713EA3969}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t>PLLF tracker</t>
   </si>
@@ -235,6 +235,15 @@
   </si>
   <si>
     <t>syntax 2: expand 1st derivative to act after any collinearity</t>
+  </si>
+  <si>
+    <t>test in v12</t>
+  </si>
+  <si>
+    <t>upversion to v12</t>
+  </si>
+  <si>
+    <t>remove first evaluation from syntax 2</t>
   </si>
 </sst>
 </file>
@@ -316,8 +325,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E42" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E42" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}" name="Table1" displayName="Table1" ref="A2:E45" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E45" xr:uid="{6516CD2F-4144-4F07-BCE6-EC520E786CB3}">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BB16AB2A-B854-4B63-A177-54B619CECB81}" name="problem" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{55DC27BD-1A0D-41AE-9DC9-2CF3279076C1}" name="Raised by" dataDxfId="3"/>
@@ -646,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C22C332-46A2-46FB-ADDE-37B0ED6C7BED}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:C42"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -700,7 +713,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -717,7 +730,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -734,7 +747,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -751,7 +764,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -768,7 +781,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -785,7 +798,7 @@
         <v>45856</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -802,7 +815,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -834,7 +847,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -851,7 +864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -868,7 +881,7 @@
         <v>45826</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -885,7 +898,7 @@
         <v>45861</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -902,7 +915,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -919,7 +932,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -936,7 +949,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -953,7 +966,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -970,7 +983,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -987,7 +1000,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1004,7 +1017,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1021,7 +1034,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -1038,7 +1051,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1055,7 +1068,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -1072,7 +1085,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -1089,7 +1102,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1106,7 +1119,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -1123,7 +1136,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -1140,7 +1153,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
@@ -1157,7 +1170,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1174,7 +1187,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
@@ -1191,7 +1204,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -1208,7 +1221,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -1225,7 +1238,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
@@ -1242,7 +1255,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -1259,7 +1272,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1276,7 +1289,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
@@ -1293,7 +1306,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
@@ -1310,7 +1323,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
@@ -1327,7 +1340,7 @@
         <v>45985</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -1337,10 +1350,14 @@
       <c r="C41" s="2">
         <v>45985</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="2">
+        <v>45994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>65</v>
       </c>
@@ -1350,8 +1367,51 @@
       <c r="C42" s="2">
         <v>45985</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="2"/>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="2">
+        <v>45994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45994</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45994</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45994</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>